<commit_message>
Bumped to 1.1.0, added link support
</commit_message>
<xml_diff>
--- a/Q Cuts CSV Template.xlsx
+++ b/Q Cuts CSV Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidheidelberger/Documents/Dev/Q-Cuts/Template Documents/Q-Cuts-Templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidheidelberger/Documents/Dev/Q-Cuts/Template Documents/Q-Cuts-CSV-Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC3BA2C4-3E84-C141-B141-402F44DF72B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B39DDE3-8099-BF46-AC81-74ACD12C5E4F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3180" yWindow="2060" windowWidth="27640" windowHeight="16940" xr2:uid="{DE285B50-AA9C-1643-AC59-3B0AF2B20F08}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
   <si>
     <t>Filename</t>
   </si>
@@ -144,9 +144,6 @@
     <t>More documentation and a full CSV tutorial can be found online</t>
   </si>
   <si>
-    <t>CSV Template Version 1.0.0</t>
-  </si>
-  <si>
     <t>Filename is case sensitive, file extension must be included.</t>
   </si>
   <si>
@@ -154,13 +151,19 @@
   </si>
   <si>
     <t>Ignore - Annoying Excel Workaround</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>CSV Template Version 1.1.0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -549,63 +552,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9A5470C-E5D8-FC47-808F-A8B151C270AA}">
-  <dimension ref="A1:Q9"/>
+  <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="F10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="41.83203125" customWidth="1"/>
-    <col min="2" max="2" width="39.5" customWidth="1"/>
-    <col min="3" max="3" width="8.5" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" customWidth="1"/>
-    <col min="5" max="8" width="21.83203125" customWidth="1"/>
-    <col min="9" max="9" width="18" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="18" customWidth="1"/>
-    <col min="12" max="17" width="6.83203125" customWidth="1"/>
+    <col min="2" max="3" width="39.5" customWidth="1"/>
+    <col min="4" max="4" width="8.5" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" customWidth="1"/>
+    <col min="6" max="9" width="21.83203125" customWidth="1"/>
+    <col min="10" max="10" width="18" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="18" customWidth="1"/>
+    <col min="13" max="18" width="6.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
-      <c r="A2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="34">
+    <row r="9" spans="1:18" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>0</v>
       </c>
@@ -613,65 +616,68 @@
         <v>1</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="F9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="G9" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="H9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I9" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="J9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K9" s="3" t="s">
+      <c r="L9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="M9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="M9" s="3" t="s">
+      <c r="N9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="N9" s="3" t="s">
+      <c r="O9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="O9" s="3" t="s">
+      <c r="P9" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="P9" s="3" t="s">
+      <c r="Q9" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="Q9" s="3" t="s">
+      <c r="R9" s="3" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="I10:I500">
+    <cfRule type="expression" dxfId="2" priority="15">
+      <formula>OR($F10="Composer",$F10="Arranger")</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="H10:H500">
-    <cfRule type="expression" dxfId="2" priority="15">
-      <formula>OR($E10="Composer",$E10="Arranger")</formula>
+    <cfRule type="expression" dxfId="1" priority="12">
+      <formula>$F10="Publisher"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10:G500">
-    <cfRule type="expression" dxfId="1" priority="12">
-      <formula>$E10="Publisher"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F10:F500">
     <cfRule type="expression" dxfId="0" priority="11">
-      <formula>$E10="Publisher"</formula>
+      <formula>$F10="Publisher"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -682,19 +688,19 @@
           <x14:formula1>
             <xm:f>Validation!$A$3:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>D501:D503</xm:sqref>
+          <xm:sqref>E501:E503</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E616B22D-26E0-2B47-A75F-31F2A29F2778}">
           <x14:formula1>
             <xm:f>Validation!$A$12:$A$14</xm:f>
           </x14:formula1>
-          <xm:sqref>E10:E503</xm:sqref>
+          <xm:sqref>F10:F503</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8693E0C9-2524-5645-8276-9A413BDDBB52}">
           <x14:formula1>
             <xm:f>Validation!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>D10:D500</xm:sqref>
+          <xm:sqref>E10:E500</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -710,13 +716,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.5" customWidth="1"/>
     <col min="2" max="2" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>20</v>
       </c>
@@ -724,7 +730,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -732,7 +738,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -740,7 +746,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -748,7 +754,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -756,7 +762,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -764,7 +770,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -772,7 +778,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -780,22 +786,22 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>22</v>
       </c>

</xml_diff>